<commit_message>
Feature Iteration and Bug Fixing ！！！
</commit_message>
<xml_diff>
--- a/UnityNamespace/src/main/resources/templates/all-namespace.xlsx
+++ b/UnityNamespace/src/main/resources/templates/all-namespace.xlsx
@@ -4,14 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="12375" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="Template" sheetId="6" r:id="rId1"/>
-    <sheet name="Label" sheetId="8" r:id="rId2"/>
-    <sheet name="Folder" sheetId="7" r:id="rId3"/>
-    <sheet name="File-timeseries" sheetId="4" r:id="rId4"/>
-    <sheet name="File-relation" sheetId="1" r:id="rId5"/>
+    <sheet name="Explanation" sheetId="16" r:id="rId1"/>
+    <sheet name="Template" sheetId="6" r:id="rId2"/>
+    <sheet name="Label" sheetId="11" r:id="rId3"/>
+    <sheet name="Folder" sheetId="7" r:id="rId4"/>
+    <sheet name="File-timeseries" sheetId="15" r:id="rId5"/>
+    <sheet name="File-relation" sheetId="1" r:id="rId6"/>
+    <sheet name="File-calculate" sheetId="12" r:id="rId7"/>
+    <sheet name="File-aggregation" sheetId="13" r:id="rId8"/>
+    <sheet name="File-reference" sheetId="14" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="51">
   <si>
     <t>name</t>
   </si>
@@ -70,19 +74,16 @@
     <t>path</t>
   </si>
   <si>
+    <t>displayName</t>
+  </si>
+  <si>
     <t>templateAlias</t>
   </si>
   <si>
-    <t>folder1/</t>
-  </si>
-  <si>
-    <t>folder1/folder2/</t>
-  </si>
-  <si>
-    <t>↓↓↓ Please enter your folder information start with row 5 ↓↓↓</t>
-  </si>
-  <si>
-    <t>mockData</t>
+    <t>folder1</t>
+  </si>
+  <si>
+    <t>folder1/folder2</t>
   </si>
   <si>
     <t>autoDashboard</t>
@@ -100,7 +101,7 @@
     <t>tag1_xxx</t>
   </si>
   <si>
-    <t>[{"name":"t0","type":"int"},{"name":"t1","type":"long"},{"name":"t2","type":"float"}]</t>
+    <t>label1,label2</t>
   </si>
   <si>
     <t>folder1/tag2</t>
@@ -109,12 +110,6 @@
     <t>tag2_xxx</t>
   </si>
   <si>
-    <t>[{"name":"t0","type":"int","index":0},{"name":"t1","type":"long","index":1},{"name":"t2","type":"float"}]</t>
-  </si>
-  <si>
-    <t>label1,label2</t>
-  </si>
-  <si>
     <t>↓↓↓ Please enter your namespace information start with row 5 ↓↓↓</t>
   </si>
   <si>
@@ -128,6 +123,72 @@
   </si>
   <si>
     <t>rel2_xxx</t>
+  </si>
+  <si>
+    <t>refers</t>
+  </si>
+  <si>
+    <t>expression</t>
+  </si>
+  <si>
+    <t>folder1/cal1</t>
+  </si>
+  <si>
+    <t>cal1_xxx</t>
+  </si>
+  <si>
+    <t>[{"name":"t0","type":"int"}]</t>
+  </si>
+  <si>
+    <t>[{"field":"t0","path":"folder1/tag1","alias":"tag1_xxx","uts":true},{"field":"t1","path":"folder1/tag2","alias":"tag2_xxx"}]</t>
+  </si>
+  <si>
+    <t>a1+a2&gt;0</t>
+  </si>
+  <si>
+    <t>folder1/cal2</t>
+  </si>
+  <si>
+    <t>cal2_xxx</t>
+  </si>
+  <si>
+    <t>[{"field":"t0","path":"folder1/tag1","alias":"tag1_xxx"},{"field":"t1","path":"folder1/tag2","alias":"tag2_xxx"}]</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>folder1/agg1</t>
+  </si>
+  <si>
+    <t>agg1_xxx</t>
+  </si>
+  <si>
+    <t>[{"path":"folder1/tag1","alias":"tag1_xxx"},{"path":"folder1/tag2","alias":"tag2_xxx"}]</t>
+  </si>
+  <si>
+    <t>5m</t>
+  </si>
+  <si>
+    <t>folder1/agg2</t>
+  </si>
+  <si>
+    <t>agg2_xxx</t>
+  </si>
+  <si>
+    <t>folder1/ref1</t>
+  </si>
+  <si>
+    <t>ref1_xxx</t>
+  </si>
+  <si>
+    <t>[{"path":"folder1/tag1","alias":"tag1_xxx"}]</t>
+  </si>
+  <si>
+    <t>folder1/ref2</t>
+  </si>
+  <si>
+    <t>ref2_xxx</t>
   </si>
 </sst>
 </file>
@@ -513,7 +574,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -547,43 +608,6 @@
         <color auto="1"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -710,7 +734,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -722,34 +746,34 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -834,7 +858,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -851,22 +875,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1181,15 +1196,31 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A5" sqref="$A5:$XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="13.875" customWidth="1"/>
     <col min="3" max="3" width="21.75" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1222,18 +1253,18 @@
         <v>6</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1244,13 +1275,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A5" sqref="$A5:$XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3"/>
@@ -1271,84 +1302,11 @@
       </c>
     </row>
     <row r="4" ht="121.5" spans="1:1">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="4"/>
-  <cols>
-    <col min="1" max="3" width="33.125" customWidth="1"/>
-    <col min="4" max="4" width="58.375" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" ht="27" spans="1:5">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" ht="27" spans="1:5">
-      <c r="A3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A4:E4"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -1357,21 +1315,20 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A5" sqref="$A5:$XFD35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="3" width="27.375" customWidth="1"/>
-    <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="14.125" customWidth="1"/>
-    <col min="9" max="9" width="14.875" customWidth="1"/>
+    <col min="1" max="4" width="33.125" customWidth="1"/>
+    <col min="5" max="5" width="58.375" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1381,83 +1338,51 @@
       <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" ht="40.5" spans="1:9">
+    </row>
+    <row r="2" ht="27" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" ht="64" customHeight="1" spans="1:9">
+      <c r="D2" s="3"/>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" ht="27" spans="1:6">
       <c r="A3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B3" s="5"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A4:F4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1470,14 +1395,17 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="$A5:$XFD30"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="3" width="33.125" customWidth="1"/>
-    <col min="4" max="4" width="58.375" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="1" max="1" width="17.4916666666667" customWidth="1"/>
+    <col min="2" max="4" width="33.125" customWidth="1"/>
+    <col min="5" max="5" width="58.375" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="14.4083333333333" customWidth="1"/>
+    <col min="8" max="8" width="14.9916666666667" customWidth="1"/>
     <col min="9" max="9" width="13.5916666666667" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1492,78 +1420,199 @@
         <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" customFormat="1" ht="27" spans="1:9">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" ht="18" customHeight="1" spans="1:9">
+      <c r="A3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="1" ht="23" customHeight="1" spans="1:9">
+      <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:I4"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="$A5:$XFD37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3"/>
+  <cols>
+    <col min="1" max="1" width="17.4916666666667" customWidth="1"/>
+    <col min="2" max="4" width="33.125" customWidth="1"/>
+    <col min="5" max="5" width="58.375" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="14.4083333333333" customWidth="1"/>
+    <col min="8" max="8" width="14.9916666666667" customWidth="1"/>
+    <col min="9" max="9" width="13.5916666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" ht="27" spans="1:9">
+    </row>
+    <row r="2" customFormat="1" ht="27" spans="1:9">
       <c r="A2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" ht="18" customHeight="1" spans="1:9">
+      <c r="A3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" ht="18" customHeight="1" spans="1:9">
-      <c r="A3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="3" t="b">
+      <c r="F3" s="6"/>
+      <c r="G3" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" ht="23" customHeight="1" spans="1:9">
-      <c r="A4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
+      <c r="I3" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="1" ht="23" customHeight="1" spans="1:9">
+      <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1573,4 +1622,368 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3"/>
+  <cols>
+    <col min="1" max="1" width="17.4916666666667" customWidth="1"/>
+    <col min="2" max="3" width="33.125" customWidth="1"/>
+    <col min="4" max="6" width="58.375" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="14.4083333333333" customWidth="1"/>
+    <col min="9" max="9" width="14.9916666666667" customWidth="1"/>
+    <col min="10" max="10" width="13.5916666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" customFormat="1" ht="40.5" spans="1:10">
+      <c r="A2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" ht="18" customHeight="1" spans="1:10">
+      <c r="A3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="1" ht="23" customHeight="1" spans="1:10">
+      <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:J4"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="$A5:$XFD35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3"/>
+  <cols>
+    <col min="1" max="1" width="17.4916666666667" customWidth="1"/>
+    <col min="2" max="3" width="33.125" customWidth="1"/>
+    <col min="4" max="4" width="58.375" customWidth="1"/>
+    <col min="5" max="5" width="18.625" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="14.4083333333333" customWidth="1"/>
+    <col min="8" max="8" width="14.9916666666667" customWidth="1"/>
+    <col min="9" max="9" width="13.5916666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" customFormat="1" ht="27" spans="1:9">
+      <c r="A2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" ht="18" customHeight="1" spans="1:9">
+      <c r="A3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="1" ht="23" customHeight="1" spans="1:9">
+      <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:I4"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="$A5:$XFD32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="17.4916666666667" customWidth="1"/>
+    <col min="2" max="3" width="33.125" customWidth="1"/>
+    <col min="4" max="4" width="58.375" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="14.4083333333333" customWidth="1"/>
+    <col min="7" max="7" width="14.9916666666667" customWidth="1"/>
+    <col min="8" max="8" width="13.5916666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" customFormat="1" spans="1:8">
+      <c r="A2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" ht="18" customHeight="1" spans="1:8">
+      <c r="A3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="1" ht="23" customHeight="1" spans="1:8">
+      <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>